<commit_message>
working namelist part B
</commit_message>
<xml_diff>
--- a/comps/A/height_setup.xlsx
+++ b/comps/A/height_setup.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="31960" windowHeight="19700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="31960" windowHeight="19700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="30m" sheetId="2" r:id="rId2"/>
+    <sheet name="50m" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>i</t>
   </si>
@@ -483,11 +484,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2046273352"/>
-        <c:axId val="2133204584"/>
+        <c:axId val="2092666312"/>
+        <c:axId val="2092669368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2046273352"/>
+        <c:axId val="2092666312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133204584"/>
+        <c:crossAx val="2092669368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133204584"/>
+        <c:axId val="2092669368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046273352"/>
+        <c:crossAx val="2092666312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -887,11 +888,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2117810440"/>
-        <c:axId val="-2117809032"/>
+        <c:axId val="2046318376"/>
+        <c:axId val="2046305272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2117810440"/>
+        <c:axId val="2046318376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117809032"/>
+        <c:crossAx val="2046305272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -908,7 +909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117809032"/>
+        <c:axId val="2046305272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117810440"/>
+        <c:crossAx val="2046318376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -969,7 +970,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$151</c:f>
+              <c:f>'30m'!$C$2:$C$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -1438,11 +1439,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115094712"/>
-        <c:axId val="-2115140632"/>
+        <c:axId val="2060095608"/>
+        <c:axId val="2060098552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115094712"/>
+        <c:axId val="2060095608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115140632"/>
+        <c:crossAx val="2060098552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1459,7 +1460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115140632"/>
+        <c:axId val="2060098552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115094712"/>
+        <c:crossAx val="2060095608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1521,7 +1522,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>'30m'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1532,7 +1533,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$212</c:f>
+              <c:f>'30m'!$B$2:$B$212</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="211"/>
@@ -1991,7 +1992,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$212</c:f>
+              <c:f>'30m'!$D$2:$D$212</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="211"/>
@@ -2458,11 +2459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2045993464"/>
-        <c:axId val="1630823496"/>
+        <c:axId val="2133134840"/>
+        <c:axId val="2133137896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2045993464"/>
+        <c:axId val="2133134840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2472,12 +2473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1630823496"/>
+        <c:crossAx val="2133137896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1630823496"/>
+        <c:axId val="2133137896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2488,7 +2489,1576 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2045993464"/>
+        <c:crossAx val="2133134840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'50m'!$C$2:$C$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="150"/>
+                <c:pt idx="0">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.242950819672131</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.448852459016393</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.654754098360656</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.860655737704918</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.066557377049181</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.272459016393443</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.478360655737704</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.684262295081967</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.89016393442623</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.096065573770492</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.301967213114754</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.507868852459016</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.71377049180328</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.91967213114754</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.125573770491803</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.331475409836065</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.537377049180328</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.74327868852459</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.949180327868852</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.155081967213116</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.360983606557378</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.56688524590164</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.772786885245901</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.978688524590163</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8.184590163934427</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8.390491803278688</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.596393442622951</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.802295081967214</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.008196721311476</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.214098360655738</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.52295081967213</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.728852459016393</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9.934754098360656</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>10.14065573770492</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>10.34655737704918</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10.55245901639344</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10.7583606557377</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10.96426229508197</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>11.17016393442623</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>11.3760655737705</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>11.58196721311475</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>11.78786885245902</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>11.99377049180328</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>12.19967213114754</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>12.4055737704918</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>12.61147540983607</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>12.81737704918033</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13.02327868852459</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>13.22918032786885</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>13.43508196721312</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>13.64098360655738</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>13.84688524590164</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>14.0527868852459</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>14.25868852459016</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>14.46459016393443</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>14.67049180327869</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>14.87639344262295</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>15.08229508196721</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>15.28819672131148</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>15.49409836065574</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>15.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2137048232"/>
+        <c:axId val="2137045848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2137048232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2137045848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2137045848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2137048232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50m'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mnt_h</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'50m'!$B$2:$B$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="211"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1050.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1150.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1350.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1450.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1650.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1850.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2150.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2350.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2450.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2550.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2600.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2650.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2700.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2850.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2900.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2950.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3150.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3200.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3300.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3350.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3450.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3550.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3650.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3850.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3950.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4050.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4100.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4150.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4200.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4300.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4350.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4400.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4450.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4600.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4650.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4700.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4800.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4850.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4900.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4950.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>5050.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>5100.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5150.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5200.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>5300.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>5350.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5400.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>5450.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5550.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>5600.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5650.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5700.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>5800.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>5850.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>5900.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5950.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>6100.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>6150.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>6200.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>6300.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6350.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>6400.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>6450.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>6550.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6600.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>6650.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>6700.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>6800.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>6850.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>6900.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6950.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>7050.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>7100.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>7150.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>7200.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>7300.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>7350.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>7400.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>7450.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'50m'!$D$2:$D$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="211"/>
+                <c:pt idx="0">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.00031706811512433</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.283085685094748</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.70852162887418</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>32.20079915208112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>61.8942032369654</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>99.53430885364453</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>143.5309752934946</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>192.0255231186256</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>242.9692557757297</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>294.210008656868</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>343.5830692629148</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>389.0026274641501</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>428.5498924580454</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>460.5541538427241</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>483.6633623068616</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>496.9012481901891</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>499.7085648887364</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>491.9667147394199</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>474.0027592868556</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>446.5756022690915</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>410.843929034673</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>368.3172568197081</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>320.7921638107719</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>270.2763910552522</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>218.9040236033926</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>168.8453341323066</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>122.2150977905816</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>80.98325158675898</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>46.89167259759539</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21.38059077685397</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.527745122859972</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.00285360821047909</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.203771491927019</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>11.46888353058092</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>31.810960879433</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>61.37063386455593</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>98.89912704876255</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>142.8110148927827</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>191.2511995080931</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>242.1732809649366</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>293.4260093301427</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>342.8441661893025</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>388.340036280213</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>427.9916049347277</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>460.1237553473726</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>483.3790354177976</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>496.7750045570465</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>499.745737789331</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>492.1657337705468</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>474.3552167074099</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>447.0666081927855</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>411.45274046691</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>369.0181539643712</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>321.5555366265492</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>271.0699901589306</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>219.6943226745641</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>169.598946263457</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>122.9001859475517</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>81.57087359339037</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>47.35700382444807</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>21.70397288039513</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5.695516530178024</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.00792666266502539</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2144822824"/>
+        <c:axId val="2144819864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2144822824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2144819864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2144819864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2144822824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2624,6 +4194,75 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4330,8 +5969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="L3" sqref="K2:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6581,7 +8220,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <f t="shared" ref="B131:B194" si="6">A131*$L$2</f>
+        <f t="shared" ref="B131:B151" si="6">A131*$L$2</f>
         <v>3900</v>
       </c>
       <c r="C131">
@@ -6923,6 +8562,2625 @@
       <c r="B151">
         <f t="shared" si="6"/>
         <v>4500</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2*$L$2</f>
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <f>3.14 + 2*3.14*MAX(0,MIN((A2-$L$3)/($L$6),1)) + 2*3.14*MAX(0,MIN((A2-$L$4)/($L$6),1))</f>
+        <v>3.14</v>
+      </c>
+      <c r="D2">
+        <f>$L$5 * 0.5 * (1 + COS(C2))</f>
+        <v>3.1706811512433042E-4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">A3*$L$2</f>
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="1">3.14 + 2*3.14*MAX(0,MIN((A3-$L$3)/($L$6),1)) + 2*3.14*MAX(0,MIN((A3-$L$4)/($L$6),1))</f>
+        <v>3.14</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="2">$L$5 * 0.5 * (1 + COS(C3))</f>
+        <v>3.1706811512433042E-4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f>2000/L2+1 - 0.5</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <f>4000/L2 + 1 - 0.5</f>
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <f>1500/L2+1 - 0.5</f>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>1150</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1450</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>1850</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>3.1706811512433042E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>3.2429508196721315</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>1.2830856850947481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>3.4488524590163934</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>11.708521628874175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>2150</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>3.6547540983606557</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>32.200799152081125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>3.860655737704918</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>61.894203236965403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>4.0665573770491807</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>99.534308853644532</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>4.2724590163934426</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>143.53097529349463</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>2350</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>4.4783606557377045</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>192.02552311862559</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>4.6842622950819672</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>242.96925577572972</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>2450</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>4.89016393442623</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>294.21000865686796</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>5.0960655737704919</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>343.58306926291482</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>2550</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>5.3019672131147537</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>389.00262746415007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>2600</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>5.5078688524590165</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>428.54989245804541</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>2650</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>5.7137704918032792</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>460.55415384272413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>5.9196721311475411</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>483.6633623068617</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>2750</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>6.125573770491803</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>496.90124819018905</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>6.3314754098360657</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>499.70856488873636</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>2850</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>6.5373770491803285</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>491.9667147394199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>6.7432786885245903</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>474.00275928685556</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>2950</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>6.9491803278688522</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>446.57560226909146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>7.1550819672131158</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>410.84392903467295</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>3050</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>7.3609836065573777</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>368.31725681970818</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>7.5668852459016396</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>320.79216381077185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>7.7727868852459014</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>270.27639105525225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>7.9786885245901633</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>218.90402360339257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>8.184590163934427</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>168.84533413230659</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B130" si="3">A67*$L$2</f>
+        <v>3300</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="4">3.14 + 2*3.14*MAX(0,MIN((A67-$L$3)/($L$6),1)) + 2*3.14*MAX(0,MIN((A67-$L$4)/($L$6),1))</f>
+        <v>8.3904918032786888</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="5">$L$5 * 0.5 * (1 + COS(C67))</f>
+        <v>122.21509779058162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="3"/>
+        <v>3350</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="4"/>
+        <v>8.5963934426229507</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>80.983251586758982</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="4"/>
+        <v>8.8022950819672143</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>46.891672597595388</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="3"/>
+        <v>3450</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="4"/>
+        <v>9.0081967213114762</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>21.380590776853975</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>3500</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="4"/>
+        <v>9.2140983606557381</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>5.5277451228599723</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>3550</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>3600</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="3"/>
+        <v>3650</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="3"/>
+        <v>3700</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="3"/>
+        <v>3750</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="3"/>
+        <v>3800</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="3"/>
+        <v>3850</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="3"/>
+        <v>3900</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="3"/>
+        <v>3950</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="3"/>
+        <v>4000</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="4"/>
+        <v>9.42</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>2.8536082104790861E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>4050</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="4"/>
+        <v>9.5229508196721309</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>1.2037714919270193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>4100</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="4"/>
+        <v>9.7288524590163927</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>11.468883530580925</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>4150</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="4"/>
+        <v>9.9347540983606564</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>31.810960879432997</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>4200</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>10.140655737704918</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>61.370633864555934</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>4250</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>10.34655737704918</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>98.899127048762551</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>4300</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="4"/>
+        <v>10.552459016393442</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>142.81101489278271</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>4350</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>10.758360655737704</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>191.25119950809315</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>4400</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>10.964262295081967</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>242.17328096493659</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>4450</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>11.170163934426229</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>293.42600933014268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>4500</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>11.376065573770491</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>342.8441661893026</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>4550</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>11.581967213114755</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>388.34003628021304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>4600</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>11.787868852459017</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>427.99160493472766</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>4650</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>11.993770491803279</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>460.12375534737259</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>4700</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>12.19967213114754</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>483.37903541779758</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>4750</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>12.405573770491802</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>496.77500455704649</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>4800</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="4"/>
+        <v>12.611475409836066</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>499.74573778933097</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>4850</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="4"/>
+        <v>12.817377049180328</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>492.16573377054681</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>4900</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="4"/>
+        <v>13.02327868852459</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>474.35521670740985</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>4950</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="4"/>
+        <v>13.229180327868853</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>447.06660819278545</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="4"/>
+        <v>13.435081967213115</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>411.45274046690997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>5050</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="4"/>
+        <v>13.640983606557377</v>
+      </c>
+      <c r="D102">
+        <f>$L$5 * 0.5 * (1 + COS(C102))</f>
+        <v>369.01815396437121</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>5100</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="4"/>
+        <v>13.846885245901639</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="5"/>
+        <v>321.55553662654921</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>5150</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="4"/>
+        <v>14.052786885245901</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="5"/>
+        <v>271.06999015893064</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>5200</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="4"/>
+        <v>14.258688524590163</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>219.69432267456415</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>5250</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="4"/>
+        <v>14.464590163934426</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>169.59894626345695</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>5300</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="4"/>
+        <v>14.67049180327869</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>122.90018594755171</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>5350</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="4"/>
+        <v>14.876393442622952</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>81.570873593390374</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>5400</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="4"/>
+        <v>15.082295081967214</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>47.357003824448071</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="3"/>
+        <v>5450</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="4"/>
+        <v>15.288196721311476</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="5"/>
+        <v>21.703972880395135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>5500</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="4"/>
+        <v>15.494098360655737</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="5"/>
+        <v>5.6955165301780237</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>5550</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>5600</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>5650</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>5700</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>5750</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>5800</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>5850</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>5900</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>5950</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="3"/>
+        <v>6050</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>6100</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="3"/>
+        <v>6150</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="3"/>
+        <v>6200</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="3"/>
+        <v>6250</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="3"/>
+        <v>6300</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="3"/>
+        <v>6350</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="3"/>
+        <v>6400</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>6450</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="4"/>
+        <v>15.7</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="5"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B151" si="6">A131*$L$2</f>
+        <v>6500</v>
+      </c>
+      <c r="C131">
+        <f t="shared" ref="C131:C151" si="7">3.14 + 2*3.14*MAX(0,MIN((A131-$L$3)/($L$6),1)) + 2*3.14*MAX(0,MIN((A131-$L$4)/($L$6),1))</f>
+        <v>15.7</v>
+      </c>
+      <c r="D131">
+        <f t="shared" ref="D131:D151" si="8">$L$5 * 0.5 * (1 + COS(C131))</f>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="6"/>
+        <v>6550</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="6"/>
+        <v>6600</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="6"/>
+        <v>6650</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="6"/>
+        <v>6700</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="6"/>
+        <v>6750</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="6"/>
+        <v>6800</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="6"/>
+        <v>6850</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="6"/>
+        <v>6900</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="6"/>
+        <v>6950</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="6"/>
+        <v>7000</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="6"/>
+        <v>7050</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="6"/>
+        <v>7100</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="6"/>
+        <v>7150</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="6"/>
+        <v>7200</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="6"/>
+        <v>7250</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="6"/>
+        <v>7300</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="6"/>
+        <v>7350</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="6"/>
+        <v>7400</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="6"/>
+        <v>7450</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="7"/>
+        <v>15.7</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="8"/>
+        <v>7.9266626650253968E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="6"/>
+        <v>7500</v>
       </c>
       <c r="C151">
         <f t="shared" si="7"/>

</xml_diff>